<commit_message>
jinding scene almost ok
</commit_message>
<xml_diff>
--- a/jinding_config_build/tmp_V04/relation.xlsx
+++ b/jinding_config_build/tmp_V04/relation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="场景内可选功能" sheetId="1" state="visible" r:id="rId2"/>
@@ -1828,25 +1828,25 @@
     <t xml:space="preserve">开</t>
   </si>
   <si>
+    <t xml:space="preserve">强功能/强功能</t>
+  </si>
+  <si>
+    <t xml:space="preserve">强功能/依赖功能</t>
+  </si>
+  <si>
+    <t xml:space="preserve">定时</t>
+  </si>
+  <si>
+    <t xml:space="preserve">温度</t>
+  </si>
+  <si>
+    <t xml:space="preserve">低</t>
+  </si>
+  <si>
+    <t xml:space="preserve">定时开:60</t>
+  </si>
+  <si>
     <t xml:space="preserve">关</t>
-  </si>
-  <si>
-    <t xml:space="preserve">强功能/强功能</t>
-  </si>
-  <si>
-    <t xml:space="preserve">强功能/依赖功能</t>
-  </si>
-  <si>
-    <t xml:space="preserve">定时</t>
-  </si>
-  <si>
-    <t xml:space="preserve">温度</t>
-  </si>
-  <si>
-    <t xml:space="preserve">低</t>
-  </si>
-  <si>
-    <t xml:space="preserve">定时开:60</t>
   </si>
   <si>
     <t xml:space="preserve">高</t>
@@ -2184,11 +2184,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.2"/>
-    <col collapsed="false" hidden="false" max="6" min="2" style="1" width="12.4279069767442"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="13.4139534883721"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="69.6511627906977"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="12.553488372093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="2" style="1" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="13.7813953488372"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="71.7441860465116"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="12.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2312,10 +2312,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="33.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.1348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.9348837209302"/>
-    <col collapsed="false" hidden="false" max="25" min="3" style="1" width="12.9209302325581"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="1" width="10.4604651162791"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.506976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.4279069767442"/>
+    <col collapsed="false" hidden="false" max="25" min="3" style="1" width="13.1674418604651"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="1" width="10.706976744186"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4159,7 +4159,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4883,14 +4883,14 @@
   </sheetPr>
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.6"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.0883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.446511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4927,19 +4927,19 @@
         <v>46</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>36</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>44</v>
@@ -4953,16 +4953,16 @@
         <v>36</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>44</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>44</v>
@@ -4979,7 +4979,7 @@
         <v>36</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>36</v>
@@ -5021,13 +5021,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.306976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>6</v>
@@ -5169,13 +5169,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.446511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>28</v>
@@ -5184,10 +5184,10 @@
         <v>27</v>
       </c>
       <c r="D1" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>50</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5198,10 +5198,10 @@
         <v>46</v>
       </c>
       <c r="C2" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>52</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>53</v>
       </c>
       <c r="E2" s="16" t="n">
         <v>28</v>
@@ -5212,7 +5212,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>54</v>
@@ -5235,7 +5235,7 @@
         <v>36</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>44</v>
@@ -5300,8 +5300,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1023" min="1" style="18" width="10.3395348837209"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1023" min="1" style="18" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5350,13 +5350,13 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L19" activeCellId="0" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.0744186046512"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>